<commit_message>
Updated team plan and added the first version of theSoftware Requirements document
</commit_message>
<xml_diff>
--- a/Project Pink/doc/Team Plan.xlsx
+++ b/Project Pink/doc/Team Plan.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="13">
   <si>
     <t>Simon Krenger</t>
   </si>
@@ -485,7 +485,7 @@
   <dimension ref="A1:AI13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Y5" sqref="Y5"/>
+      <selection activeCell="Q6" sqref="Q6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -787,12 +787,24 @@
       <c r="I6" s="4"/>
       <c r="J6" s="5"/>
       <c r="K6" s="5"/>
-      <c r="L6" s="4"/>
-      <c r="M6" s="4"/>
-      <c r="N6" s="4"/>
-      <c r="O6" s="4"/>
-      <c r="P6" s="4"/>
-      <c r="Q6" s="4"/>
+      <c r="L6" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="M6" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="N6" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="O6" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="P6" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="Q6" s="4" t="s">
+        <v>8</v>
+      </c>
       <c r="R6" s="4"/>
       <c r="S6" s="4"/>
       <c r="T6" s="5"/>
@@ -810,7 +822,7 @@
       <c r="AF6" s="4"/>
       <c r="AG6" s="4"/>
       <c r="AI6">
-        <v>0</v>
+        <v>6</v>
       </c>
     </row>
     <row r="7" spans="1:35">
@@ -910,27 +922,27 @@
       </c>
       <c r="L9">
         <f t="shared" si="14"/>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="M9">
         <f t="shared" si="14"/>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="N9">
         <f t="shared" si="14"/>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="O9">
         <f t="shared" si="14"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="P9">
         <f t="shared" si="14"/>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="Q9">
         <f t="shared" si="14"/>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="R9">
         <f t="shared" si="14"/>

</xml_diff>